<commit_message>
Dane przykladowe dla pierwszych 20 atrybutow.
git-svn-id: https://localhost:8443/svn/bdr@985 5173494c-6dae-45e1-bfb1-e08744c75a4d
</commit_message>
<xml_diff>
--- a/TPP/dokumenty/TPP_atrybuty.xlsx
+++ b/TPP/dokumenty/TPP_atrybuty.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="129">
   <si>
     <t>Spowolnienie</t>
   </si>
@@ -478,13 +478,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,8 +789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,12 +1776,424 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>34</v>
+      </c>
+      <c r="F4" s="6">
+        <v>2</v>
+      </c>
+      <c r="G4" s="6">
+        <v>31</v>
+      </c>
+      <c r="H4" s="6">
+        <v>2</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="J4" s="6">
+        <v>1</v>
+      </c>
+      <c r="K4" s="6">
+        <v>0</v>
+      </c>
+      <c r="L4" s="6">
+        <v>1</v>
+      </c>
+      <c r="M4" s="6">
+        <v>1</v>
+      </c>
+      <c r="N4" s="6">
+        <v>1</v>
+      </c>
+      <c r="O4" s="6">
+        <v>1</v>
+      </c>
+      <c r="P4" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>1</v>
+      </c>
+      <c r="R4" s="6">
+        <v>1</v>
+      </c>
+      <c r="S4" s="6">
+        <v>10</v>
+      </c>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>35</v>
+      </c>
+      <c r="F5" s="6">
+        <v>3</v>
+      </c>
+      <c r="G5" s="6">
+        <v>31</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="J5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
+        <v>0</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6">
+        <v>0</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6">
+        <v>1</v>
+      </c>
+      <c r="S5" s="6">
+        <v>10</v>
+      </c>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6">
+        <v>2</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
+        <v>59</v>
+      </c>
+      <c r="F6" s="6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>57</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="6">
+        <v>1</v>
+      </c>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6">
+        <v>1</v>
+      </c>
+      <c r="O6" s="6">
+        <v>0</v>
+      </c>
+      <c r="P6" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>2</v>
+      </c>
+      <c r="R6" s="6">
+        <v>0</v>
+      </c>
+      <c r="S6" s="6">
+        <v>15</v>
+      </c>
+      <c r="T6" s="6">
+        <v>20</v>
+      </c>
+      <c r="U6" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>60</v>
+      </c>
+      <c r="F7" s="6">
+        <v>3</v>
+      </c>
+      <c r="G7" s="6">
+        <v>57</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6">
+        <v>1</v>
+      </c>
+      <c r="J7" s="6">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6">
+        <v>0</v>
+      </c>
+      <c r="L7" s="6">
+        <v>1</v>
+      </c>
+      <c r="M7" s="6">
+        <v>1</v>
+      </c>
+      <c r="N7" s="6">
+        <v>1</v>
+      </c>
+      <c r="O7" s="6">
+        <v>1</v>
+      </c>
+      <c r="P7" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>2</v>
+      </c>
+      <c r="R7" s="6">
+        <v>1</v>
+      </c>
+      <c r="S7" s="6">
+        <v>15</v>
+      </c>
+      <c r="T7" s="6">
+        <v>20</v>
+      </c>
+      <c r="U7" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>70</v>
+      </c>
+      <c r="F8" s="6">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6">
+        <v>69</v>
+      </c>
+      <c r="H8" s="6">
+        <v>4</v>
+      </c>
+      <c r="I8" s="6">
+        <v>0</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
+        <v>0</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6">
+        <v>0</v>
+      </c>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6">
+        <v>0</v>
+      </c>
+      <c r="S8" s="6">
+        <v>0</v>
+      </c>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="6"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="6"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Atrybuty - wersja nieobrobiona; ze spotkania.
git-svn-id: https://localhost:8443/svn/bdr@988 5173494c-6dae-45e1-bfb1-e08744c75a4d
</commit_message>
<xml_diff>
--- a/TPP/dokumenty/TPP_atrybuty.xlsx
+++ b/TPP/dokumenty/TPP_atrybuty.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="546"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="214">
   <si>
     <t>Spowolnienie</t>
   </si>
@@ -45,39 +45,24 @@
     <t xml:space="preserve">Wizyta </t>
   </si>
   <si>
-    <t>0=przedoperacyjna, 1=1 rok po DBS, 2=2lata po DBS, 3=3lata po DBS, 4=4 lata po DBS, 5=5 lat po DBS</t>
-  </si>
-  <si>
     <t>int</t>
   </si>
   <si>
-    <t>(może być też np. imię i nazwisko lub inne dane osobowe - nie będziemy wówczas zapisywać takiego ID a jedynie jego hash, aby identyfikować/weryfikować badanie z pacjentem)</t>
-  </si>
-  <si>
     <t>[0=kobieta, 1=mężczyzna]</t>
   </si>
   <si>
-    <t xml:space="preserve"> [1=drżenie, 2=sztywność, 3=spowolnienie, 4=inne (nie dyskinezy i fluktuacje)]</t>
-  </si>
-  <si>
     <t>bit</t>
   </si>
   <si>
     <t>// ta i poniższa - wyznaczniki przydatności zabiegu</t>
   </si>
   <si>
-    <t>[3=amantadyna, 4=MAOBinh, 5=COMTinh, 6=cholinolityk, 7=inne]</t>
-  </si>
-  <si>
     <t>czy to zawsze będzie max. 1 lek, czy też rozbić na 5 osobnych atrybutów? Czy potrzebujemy też informacji o ich dawkach dobowych?</t>
   </si>
   <si>
     <t>[1=zaburzenia równowagi, 2=spowolnienie, 3=sztywność, 4=drżenie, 5=otępienie, 6=dyskinezy i fluktuacje, 7=objawy autonomiczne, 8=inne]</t>
   </si>
   <si>
-    <t>[1=zaparcia, 2=objawy dyzuryczne, 3=hipotonia ortostatyczna, 4=nadmierna potliwość, 5=ślinotok, 6=łojotok, 0=brak]</t>
-  </si>
-  <si>
     <t xml:space="preserve">RLS </t>
   </si>
   <si>
@@ -90,9 +75,6 @@
     <t>Czy wszystkie atrybuty z typem bit obejdą się z dwiema wartościami, czy lepiej zmienić któryś na wyliczenie, by była możliwa jeszcze jedna lub większa liczba dalszych opcji?</t>
   </si>
   <si>
-    <t>[1=TAK, 0=NIE, 2=MCI]</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dyzartria </t>
   </si>
   <si>
@@ -120,9 +102,6 @@
     <t>Posturografia</t>
   </si>
   <si>
-    <t>[1=TAK, 0=NIE, 2=DATSCAN]</t>
-  </si>
-  <si>
     <t>Wiek</t>
   </si>
   <si>
@@ -276,9 +255,6 @@
     <t>UPDRS_31_on</t>
   </si>
   <si>
-    <t>Okulografia_on</t>
-  </si>
-  <si>
     <t>UPDRS_I_off</t>
   </si>
   <si>
@@ -330,9 +306,6 @@
     <t>UPDRS_31_off</t>
   </si>
   <si>
-    <t>Okulografia_off</t>
-  </si>
-  <si>
     <t>HY_off</t>
   </si>
   <si>
@@ -360,15 +333,6 @@
     <t>USGsrodmozgowia</t>
   </si>
   <si>
-    <t xml:space="preserve">ScyntygrafiaMozgu </t>
-  </si>
-  <si>
-    <t>ZapisDrżenia</t>
-  </si>
-  <si>
-    <t>BadWechu</t>
-  </si>
-  <si>
     <t>WynikWechu</t>
   </si>
   <si>
@@ -403,6 +367,297 @@
   </si>
   <si>
     <t>UPDRS_IV_on</t>
+  </si>
+  <si>
+    <t>NumerPacjenta</t>
+  </si>
+  <si>
+    <t>varchar(20)</t>
+  </si>
+  <si>
+    <t>rok i miesiąc urodzenia pacjenta - wprowadzany do bazy;</t>
+  </si>
+  <si>
+    <t>jako wyliczalny z dokładnością</t>
+  </si>
+  <si>
+    <t>0=przedoperacyjna, 0,5=po pół roku; 1=1 rok po DBS, 2=2lata po DBS, 3=3lata po DBS, 4=4 lata po DBS, 5=5 lat po DBS</t>
+  </si>
+  <si>
+    <t>rok i miesiąc</t>
+  </si>
+  <si>
+    <t>Objawy inne</t>
+  </si>
+  <si>
+    <t>varchar(50)</t>
+  </si>
+  <si>
+    <t>varchar(80)</t>
+  </si>
+  <si>
+    <t>wypełniane gdy zaznaczono inne;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [1=drżenie, 2=sztywność, 3=spowolnienie, 4=inne (nie dyskinezy i fluktuacje)]  - do usunięcia</t>
+  </si>
+  <si>
+    <t>Pierwszy objaw</t>
+  </si>
+  <si>
+    <t>wartości od 1 do 8;</t>
+  </si>
+  <si>
+    <t>DyskinezyOdPoczatkuChoroby</t>
+  </si>
+  <si>
+    <t>FluktuacjeOdPoczatkuChoroby</t>
+  </si>
+  <si>
+    <t>podawany w minutach</t>
+  </si>
+  <si>
+    <t>jeśli zaznaczono inne</t>
+  </si>
+  <si>
+    <t>Wszystkie pola typu BIT - zmienić na 0/1/2 (b/d)</t>
+  </si>
+  <si>
+    <t>[3=amantadyna, 4=MAOBinh, 5=COMTinh, 6=cholinolityk, 7=inne] - zamienić na binarne; podobnie jak przy objawach; gdy zaznaczono - opcja wpisania dawki</t>
+  </si>
+  <si>
+    <t>LekiInneJakie</t>
+  </si>
+  <si>
+    <t>zostawiamy jeden</t>
+  </si>
+  <si>
+    <t>DominującyObjawUwagi</t>
+  </si>
+  <si>
+    <t>dostępne niezależnie od zaznaczenia ww.</t>
+  </si>
+  <si>
+    <t>[1=zaparcia, 2=objawy dyzuryczne, 3=hipotonia ortostatyczna, 4=nadmierna potliwość, 5=ślinotok, 6=łojotok, 0=brak] - zamienić na "binarne"</t>
+  </si>
+  <si>
+    <t>ObjawyAutonomiczneFormularz</t>
+  </si>
+  <si>
+    <t>TABLE</t>
+  </si>
+  <si>
+    <t>opcjonalnie; wg. Dostarczonego formularza</t>
+  </si>
+  <si>
+    <t>[1=TAK, 0,5=częściowo, 0=NIE, 2=brak, danych]</t>
+  </si>
+  <si>
+    <t>&lt;wstawić ankieta od 25 do 34)</t>
+  </si>
+  <si>
+    <t>LimitDysfagii</t>
+  </si>
+  <si>
+    <t>uzupełnić - zob. wydruk formularza</t>
+  </si>
+  <si>
+    <t>rozbić na 4 wg. DBS; na tabele UPDRS - badanie wg DBS dotyczy tylko follow-up</t>
+  </si>
+  <si>
+    <t>USGWynik</t>
+  </si>
+  <si>
+    <t>PDQ39</t>
+  </si>
+  <si>
+    <t>AIMS</t>
+  </si>
+  <si>
+    <t>Epworth</t>
+  </si>
+  <si>
+    <t>CGI</t>
+  </si>
+  <si>
+    <t>TestZegara</t>
+  </si>
+  <si>
+    <t>MMSE</t>
+  </si>
+  <si>
+    <t>0-30</t>
+  </si>
+  <si>
+    <t>psychologiczne - start</t>
+  </si>
+  <si>
+    <t>WAIS-R_Wiadomosci</t>
+  </si>
+  <si>
+    <t>WAIS-R_PowtarzanieCyfr</t>
+  </si>
+  <si>
+    <t>może się zmienić/rozszerzyć zestaw kryteriów</t>
+  </si>
+  <si>
+    <t>SkalaDepresjiBecka</t>
+  </si>
+  <si>
+    <t>TestFluencjiZwierzeta</t>
+  </si>
+  <si>
+    <t>TestFluencjiOstre</t>
+  </si>
+  <si>
+    <t>TestFluencjiK</t>
+  </si>
+  <si>
+    <t>TestLaczeniaPunktowA</t>
+  </si>
+  <si>
+    <t>TestLaczeniaPunktowB</t>
+  </si>
+  <si>
+    <t>TestUczeniaSlownoSluchowego</t>
+  </si>
+  <si>
+    <t>TestStroopa</t>
+  </si>
+  <si>
+    <t>TestMinnesota</t>
+  </si>
+  <si>
+    <t>psychologiczne - koniec</t>
+  </si>
+  <si>
+    <t>Wideo</t>
+  </si>
+  <si>
+    <t>TestSchodkowy</t>
+  </si>
+  <si>
+    <t>TestSchodkowyCzas1</t>
+  </si>
+  <si>
+    <t>TestSchodkowyCzas2</t>
+  </si>
+  <si>
+    <t>TestSchodkowyŚrednia-wylczalna</t>
+  </si>
+  <si>
+    <t>decimal(4,2)</t>
+  </si>
+  <si>
+    <t>TestMarszu</t>
+  </si>
+  <si>
+    <t>bin</t>
+  </si>
+  <si>
+    <t>TestMarszuCzas1</t>
+  </si>
+  <si>
+    <t>TestMarszuCzas2</t>
+  </si>
+  <si>
+    <t>Okulografia</t>
+  </si>
+  <si>
+    <t>RejestracjaMowy</t>
+  </si>
+  <si>
+    <t>Tremorometria</t>
+  </si>
+  <si>
+    <t>testy równoważne</t>
+  </si>
+  <si>
+    <t>równoważne - start</t>
+  </si>
+  <si>
+    <t>UpAndGo</t>
+  </si>
+  <si>
+    <t>UpAndGoLiczby</t>
+  </si>
+  <si>
+    <t>UpAndGoKubekPrawa</t>
+  </si>
+  <si>
+    <t>UpAndGoKubekLewa</t>
+  </si>
+  <si>
+    <t>TST</t>
+  </si>
+  <si>
+    <t>decimal(3,1)</t>
+  </si>
+  <si>
+    <t>TandemPivot</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>WTT</t>
+  </si>
+  <si>
+    <t>sekundy</t>
+  </si>
+  <si>
+    <t>równoważne - end</t>
+  </si>
+  <si>
+    <t>Holter</t>
+  </si>
+  <si>
+    <t>pH-metriaPrzełyku</t>
+  </si>
+  <si>
+    <t>SPECT</t>
+  </si>
+  <si>
+    <t>MRI</t>
+  </si>
+  <si>
+    <t>MRIwynik</t>
+  </si>
+  <si>
+    <t>zastąpić: wartości binarne, plus tekstowy dla "inne"</t>
+  </si>
+  <si>
+    <t>0=brak okna; 1=brak hyperechogeniczności; 2=hyperechgeniczność</t>
+  </si>
+  <si>
+    <t>Genetyka</t>
+  </si>
+  <si>
+    <t>GenetykaWynik</t>
+  </si>
+  <si>
+    <t>Surowica</t>
+  </si>
+  <si>
+    <t>SurowicaPozostało</t>
+  </si>
+  <si>
+    <t>Masa</t>
+  </si>
+  <si>
+    <t>Rodzinnosc</t>
+  </si>
+  <si>
+    <t>decimal(4,1)</t>
+  </si>
+  <si>
+    <t>Wykształcenie</t>
+  </si>
+  <si>
+    <t>podst=1/zaw/średnie/wyższe</t>
+  </si>
+  <si>
+    <t>do 8 kombinacji; LatencyMeter/JazzNovo</t>
   </si>
 </sst>
 </file>
@@ -451,7 +706,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -474,11 +729,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -486,6 +752,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,45 +1054,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D100"/>
+  <dimension ref="A1:D161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:D30"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" customWidth="1"/>
     <col min="3" max="3" width="124.28515625" customWidth="1"/>
     <col min="4" max="4" width="159" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>121</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -844,928 +1117,1555 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>110</v>
-      </c>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>121</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>36</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>39</v>
+        <v>208</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>40</v>
+        <v>209</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>52</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>41</v>
+        <v>211</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
-        <v>61</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>120</v>
+      </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>122</v>
+      </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>129</v>
+      </c>
       <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2" t="s">
-        <v>15</v>
+        <v>101</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="D23" s="2" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C25" s="2"/>
-      <c r="D25" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="D25" s="2"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C26" s="2"/>
-      <c r="D26" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>49</v>
+        <v>123</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>17</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>18</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>56</v>
+        <v>130</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>57</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>20</v>
+        <v>131</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>14</v>
+        <v>102</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="2" t="s">
-        <v>62</v>
-      </c>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C37" s="2"/>
-      <c r="D37" s="2"/>
+      <c r="D37" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C38" s="2"/>
-      <c r="D38" s="2"/>
+      <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="2" t="s">
-        <v>27</v>
+        <v>101</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
+        <v>125</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>14</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="2" t="s">
-        <v>65</v>
-      </c>
+      <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D42" s="2"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>105</v>
+        <v>138</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2" t="s">
-        <v>68</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>106</v>
+        <v>49</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" s="2"/>
-      <c r="D45" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>87</v>
+        <v>141</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C46" s="2"/>
-      <c r="D46" s="2"/>
+        <v>142</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="D47" s="2" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>126</v>
+        <v>16</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>90</v>
+        <v>52</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" s="2"/>
+        <v>102</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>144</v>
+      </c>
       <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>91</v>
+        <v>19</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>92</v>
+        <v>20</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>127</v>
+        <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
+      <c r="D54" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>93</v>
+        <v>56</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
+      <c r="D56" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>95</v>
+        <v>59</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C57" s="2"/>
+        <v>11</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="D59" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>110</v>
-      </c>
+      <c r="A60" s="2"/>
+      <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C61" s="2"/>
-      <c r="D61" s="2"/>
+      <c r="D61" s="2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C68" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>148</v>
+      </c>
       <c r="D68" s="2"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C70" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D70" s="2"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C71" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D71" s="2"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C72" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C73" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D73" s="2"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C74" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D74" s="2"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C75" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D75" s="2"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C76" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>77</v>
+        <v>90</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C77" s="2"/>
+        <v>101</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="D77" s="2"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C86" s="2"/>
       <c r="D86" s="2"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>114</v>
+        <v>65</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C87" s="2"/>
       <c r="D87" s="2"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C88" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C88" s="2"/>
       <c r="D88" s="2"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>86</v>
+        <v>67</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>29</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C89" s="2"/>
       <c r="D89" s="2"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>33</v>
+        <v>98</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>29</v>
+        <v>147</v>
       </c>
       <c r="D90" s="2"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>29</v>
+        <v>147</v>
       </c>
       <c r="D91" s="2"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>29</v>
+        <v>147</v>
       </c>
       <c r="D92" s="2"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>117</v>
+        <v>69</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2" t="s">
-        <v>30</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>118</v>
+        <v>70</v>
       </c>
       <c r="B94" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D94" s="2"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D95" s="2"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D96" s="2"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D97" s="2"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C98" s="2"/>
+      <c r="D98" s="2"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C99" s="2"/>
+      <c r="D99" s="2"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C103" s="2"/>
+      <c r="D103" s="2"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C104" s="2"/>
+      <c r="D104" s="2"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C105" s="2"/>
+      <c r="D105" s="2"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C106" s="2"/>
+      <c r="D106" s="2"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D107" s="2"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C108" s="2"/>
+      <c r="D108" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D110" s="2"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C111" s="2"/>
+      <c r="D111" s="2"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C112" s="2"/>
+      <c r="D112" s="2"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C115" s="2"/>
+      <c r="D115" s="2"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C117" s="2"/>
+      <c r="D117" s="2"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C118" s="2"/>
+      <c r="D118" s="2"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D119" s="2"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C120" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D120" s="2"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C121" s="6"/>
+      <c r="D121" s="2"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C122" s="6"/>
+      <c r="D122" s="2"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C123" s="6"/>
+      <c r="D123" s="2"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C124" s="6"/>
+      <c r="D124" s="2"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C125" s="6"/>
+      <c r="D125" s="2"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C126" s="6"/>
+      <c r="D126" s="2"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B127" s="2"/>
+      <c r="D127" s="2"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C128" s="2"/>
+      <c r="D128" s="2"/>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C129" s="2"/>
+      <c r="D129" s="2"/>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C130" s="2"/>
+      <c r="D130" s="2"/>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B132" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C132" s="2"/>
+      <c r="D132" s="2"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C133" s="2"/>
+      <c r="D133" s="2"/>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C134" s="2"/>
+      <c r="D134" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C135" s="2"/>
+      <c r="D135" s="2"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D136" s="2"/>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D137" s="2"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C139" s="2"/>
+      <c r="D139" s="2"/>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="B140" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C140" s="2"/>
+      <c r="D140" s="2"/>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C141" s="2"/>
+      <c r="D141" s="2"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B142" s="7"/>
+      <c r="C142" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D142" s="2"/>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D143" s="2"/>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D144" s="2"/>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C145" s="2"/>
+      <c r="D145" s="2"/>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B146" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C146" s="2"/>
+      <c r="D146" s="2"/>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B147" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C147" s="2"/>
+      <c r="D147" s="2"/>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B148" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C148" s="2"/>
+      <c r="D148" s="2"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" s="2"/>
+      <c r="B149" s="2"/>
+      <c r="C149" s="2"/>
+      <c r="D149" s="2"/>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" s="2"/>
+      <c r="B150" s="2"/>
+      <c r="C150" s="2"/>
+      <c r="D150" s="2"/>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D151" s="2"/>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" s="2"/>
+      <c r="B152" s="2"/>
+      <c r="C152" s="2"/>
+      <c r="D152" s="2"/>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" s="2"/>
+      <c r="B153" s="2"/>
+      <c r="C153" s="2"/>
+      <c r="D153" s="2"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C158" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C94" s="2"/>
-      <c r="D94" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C97" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C98" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C99" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C100" s="5" t="s">
-        <v>125</v>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C159" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C160" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C161" s="5" t="s">
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1778,7 +2678,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -1793,64 +2693,64 @@
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="6" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>35</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>42</v>
       </c>
       <c r="K3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="L3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="S3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="O3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="P3" s="6" t="s">
+      <c r="U3" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="Q3" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="R3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="S3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="T3" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="U3" s="6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">

</xml_diff>